<commit_message>
test class for Volume Prediction
</commit_message>
<xml_diff>
--- a/MonitoringLayer/testdata/volumePrediction/results.xlsx
+++ b/MonitoringLayer/testdata/volumePrediction/results.xlsx
@@ -1201,20 +1201,274 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="37"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="43"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="65"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="67"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="75"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="76"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="87"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="95"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="97"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$6:$D$105</c:f>
@@ -1536,11 +1790,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="409131944"/>
-        <c:axId val="409128416"/>
+        <c:axId val="175878856"/>
+        <c:axId val="175878464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="409131944"/>
+        <c:axId val="175878856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409128416"/>
+        <c:crossAx val="175878464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1614,7 +1868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="409128416"/>
+        <c:axId val="175878464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130000"/>
@@ -1659,7 +1913,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1678,7 +1932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409131944"/>
+        <c:crossAx val="175878856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2860,20 +3114,179 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="33"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="42"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="56"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="82"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="94"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="96"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$20:$H$119</c:f>
@@ -3195,11 +3608,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="409730032"/>
-        <c:axId val="409728072"/>
+        <c:axId val="175877288"/>
+        <c:axId val="175876896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="409730032"/>
+        <c:axId val="175877288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,7 +3678,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409728072"/>
+        <c:crossAx val="175876896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3273,7 +3686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="409728072"/>
+        <c:axId val="175876896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600000"/>
@@ -3306,7 +3719,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3325,7 +3738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409730032"/>
+        <c:crossAx val="175877288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4872,49 +5285,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S150" sqref="S150"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>